<commit_message>
Save_all tests for Supplier and StorageLocation ExcelController
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/storageLocationsOk.xlsx
+++ b/src/test/resources/excelTests/storageLocationsOk.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>KARAKAS</t>
+  </si>
+  <si>
+    <t>EX99</t>
+  </si>
+  <si>
+    <t>TEST SL</t>
+  </si>
+  <si>
+    <t>EX101</t>
   </si>
 </sst>
 </file>
@@ -109,7 +118,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -222,11 +231,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -250,6 +287,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -530,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,16 +685,40 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4" t="str">
+      <c r="D10" s="11" t="str">
         <f>IF(TRUE,C5,B3)</f>
         <v>BUENOS</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>